<commit_message>
fixed bugs regarding different scenarios handling for searchv2
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\Etna\resources\ExcelsheetData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\template\resources\ExcelsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,16 +16,17 @@
     <sheet name="keyword_ExactMatch_BNOrUPC" sheetId="2" r:id="rId2"/>
     <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId3"/>
     <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId4"/>
-    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId5"/>
-    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId6"/>
-    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId7"/>
+    <sheet name="keyword_ExactMatching_PNOrUPC" sheetId="8" r:id="rId5"/>
+    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId6"/>
+    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId7"/>
+    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -36,101 +37,116 @@
     <t>Part Number Or MPN</t>
   </si>
   <si>
-    <t>8677596_1 SP-CVL-3X</t>
-  </si>
-  <si>
-    <t>8494640 SP-CVL-4X</t>
-  </si>
-  <si>
-    <t>11387288 15003</t>
-  </si>
-  <si>
     <t>Brand Name Or UPC</t>
   </si>
   <si>
-    <t>MiraCool® 048615965734</t>
-  </si>
-  <si>
-    <t>Buffalo™ 048615965727</t>
-  </si>
-  <si>
-    <t>Trimaco 048615965383</t>
-  </si>
-  <si>
     <t>Brand Name Or Part Number</t>
   </si>
   <si>
-    <t>MiraCool® 8494640</t>
-  </si>
-  <si>
-    <t>Buffalo™ 8677596_1</t>
-  </si>
-  <si>
-    <t>Trimaco 8494640_2</t>
-  </si>
-  <si>
     <t>Brand Name Or MPN</t>
   </si>
   <si>
-    <t>MiraCool® 15010</t>
-  </si>
-  <si>
-    <t>Markal® 837-REG-3XL-NAY</t>
-  </si>
-  <si>
     <t>MPN</t>
   </si>
   <si>
     <t>TC_Searchv2_001</t>
   </si>
   <si>
-    <t>SP-CVL-2X</t>
-  </si>
-  <si>
-    <t>SP-CVL-3X</t>
-  </si>
-  <si>
-    <t>SP-CVL-4X</t>
-  </si>
-  <si>
     <t>Part Number</t>
   </si>
   <si>
     <t>UPC</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>048615965734</t>
-  </si>
-  <si>
-    <t>048615965727</t>
-  </si>
-  <si>
-    <t>user name</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>webuser@unilogcorp.com</t>
-  </si>
-  <si>
-    <t>11387286</t>
-  </si>
-  <si>
-    <t>11387287</t>
-  </si>
-  <si>
-    <t>11387288</t>
+    <t>1607</t>
+  </si>
+  <si>
+    <t>168867</t>
+  </si>
+  <si>
+    <t>13861</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>K-7272-CP</t>
+  </si>
+  <si>
+    <t>ELEGANCIA7242C10WHT</t>
+  </si>
+  <si>
+    <t>K-7104-BN</t>
+  </si>
+  <si>
+    <t>034449658003</t>
+  </si>
+  <si>
+    <t>650531536877</t>
+  </si>
+  <si>
+    <t>087206579400</t>
+  </si>
+  <si>
+    <t>168867 K-7272-BRZ</t>
+  </si>
+  <si>
+    <t>678910 TestMPN</t>
+  </si>
+  <si>
+    <t>12345 K-7104-BN</t>
+  </si>
+  <si>
+    <t>12345 Test1234</t>
+  </si>
+  <si>
+    <t>Kohler  304731</t>
+  </si>
+  <si>
+    <t>Brizo 12345</t>
+  </si>
+  <si>
+    <t>Charman test1234</t>
+  </si>
+  <si>
+    <t>Nutone TestUPC</t>
+  </si>
+  <si>
+    <t>3m 650531846716</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>3M TestMPN</t>
+  </si>
+  <si>
+    <t>Brizo TestMPN</t>
+  </si>
+  <si>
+    <t>Part Number or UPC</t>
+  </si>
+  <si>
+    <t>1607 034449574501</t>
+  </si>
+  <si>
+    <t>304731 TestUPC</t>
+  </si>
+  <si>
+    <t>678910 847877043767</t>
+  </si>
+  <si>
+    <t>12345 TestUPC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -151,8 +167,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000038"/>
-      <name val="Roboto-Regular"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -223,20 +240,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1397,75 +1415,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IJ4"/>
+  <dimension ref="A1:IH5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="244" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
+    <col min="3" max="242" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="B2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="B3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>5</v>
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1479,74 +1479,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1557,74 +1529,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="B3" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1635,60 +1581,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
+      <c r="B3" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1698,74 +1624,168 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="B1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
-        <v>18</v>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1773,154 +1793,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bugs regarding exact matching
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="keyword_ExactMatch_PNOrMPN" sheetId="1" r:id="rId1"/>
     <sheet name="keyword_ExactMatch_BNOrUPC" sheetId="2" r:id="rId2"/>
     <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId3"/>
     <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId4"/>
-    <sheet name="keyword_ExactMatching_PNOrUPC" sheetId="8" r:id="rId5"/>
+    <sheet name="keyword_ExactMatching_UPCOrPN" sheetId="8" r:id="rId5"/>
     <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId6"/>
     <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId7"/>
     <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId8"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -88,58 +88,43 @@
     <t>087206579400</t>
   </si>
   <si>
-    <t>168867 K-7272-BRZ</t>
-  </si>
-  <si>
-    <t>678910 TestMPN</t>
-  </si>
-  <si>
-    <t>12345 K-7104-BN</t>
-  </si>
-  <si>
-    <t>12345 Test1234</t>
-  </si>
-  <si>
-    <t>Kohler  304731</t>
-  </si>
-  <si>
-    <t>Brizo 12345</t>
-  </si>
-  <si>
-    <t>Charman test1234</t>
-  </si>
-  <si>
-    <t>Nutone TestUPC</t>
-  </si>
-  <si>
-    <t>3m 650531846716</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>3M TestMPN</t>
-  </si>
-  <si>
-    <t>Brizo TestMPN</t>
-  </si>
-  <si>
     <t>Part Number or UPC</t>
   </si>
   <si>
-    <t>1607 034449574501</t>
-  </si>
-  <si>
-    <t>304731 TestUPC</t>
-  </si>
-  <si>
-    <t>678910 847877043767</t>
-  </si>
-  <si>
-    <t>12345 TestUPC</t>
+    <t>BainUltra ELEGANCIA7242C10BIS</t>
+  </si>
+  <si>
+    <t>ELEGANCIA7242C10WHT ELEGANCIA7242C10WHT</t>
+  </si>
+  <si>
+    <t>13861 K-7272-CP</t>
+  </si>
+  <si>
+    <t>Brizo 63003LF-RB</t>
+  </si>
+  <si>
+    <t>Nutone 026715145096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moen 026508161012 </t>
+  </si>
+  <si>
+    <t>Moen 026508161029</t>
+  </si>
+  <si>
+    <t>847877043767 800-12-B2-24</t>
+  </si>
+  <si>
+    <t>034449574501 T11800</t>
+  </si>
+  <si>
+    <t>TestUPC 12345</t>
   </si>
 </sst>
 </file>
@@ -240,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -250,11 +235,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,57 +1401,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IH5"/>
+  <dimension ref="A1:IH3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="1" customWidth="1"/>
     <col min="3" max="242" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1479,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,21 +1473,29 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1529,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,23 +1531,7 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1581,16 +1543,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1605,29 +1567,22 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>32</v>
+      <c r="B2" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,40 +1595,32 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>33</v>
+      <c r="B1" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>34</v>
+      <c r="B2" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>35</v>
+      <c r="B3" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>37</v>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +1655,7 @@
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1716,7 +1663,7 @@
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1724,7 +1671,7 @@
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1819,7 +1766,7 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated selenium version, added implicitly wait for ie driver, completed OR condition and started AND condition
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="keyword_ExactMatch_PNOrMPN" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,23 @@
     <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId3"/>
     <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId4"/>
     <sheet name="keyword_ExactMatching_UPCOrPN" sheetId="8" r:id="rId5"/>
-    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId6"/>
-    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId7"/>
-    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId8"/>
+    <sheet name="keyword_OrCond_BrandNameOrMPN" sheetId="9" r:id="rId6"/>
+    <sheet name="keyword_OrCond_PNOrMPN" sheetId="10" r:id="rId7"/>
+    <sheet name="keyword_OrCond_BNOrPN" sheetId="12" r:id="rId8"/>
+    <sheet name="keyword_OrCond_MPNOrPN" sheetId="13" r:id="rId9"/>
+    <sheet name="keyword_OrCond_PNOrUPC" sheetId="14" r:id="rId10"/>
+    <sheet name="keyword_AndCond_BNAndMPN" sheetId="16" r:id="rId11"/>
+    <sheet name="keyword_OrCond_BNOrUPC" sheetId="15" r:id="rId12"/>
+    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId13"/>
+    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId14"/>
+    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -125,6 +132,72 @@
   </si>
   <si>
     <t>TestUPC 12345</t>
+  </si>
+  <si>
+    <t>BrandName or MPN</t>
+  </si>
+  <si>
+    <t>Gerber OR 649NS</t>
+  </si>
+  <si>
+    <t>Jones Stephens OR ELEGANCIA7242C10WHT</t>
+  </si>
+  <si>
+    <t>Aquatic  OR  2603-CTSR</t>
+  </si>
+  <si>
+    <t>12584BIS OR T6620ORB</t>
+  </si>
+  <si>
+    <t>JBC101 OR 741WHNT</t>
+  </si>
+  <si>
+    <t>Jones Stephens OR K6589-U-96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquatic OR 2603CTSRWHT </t>
+  </si>
+  <si>
+    <t>BrandName or PN</t>
+  </si>
+  <si>
+    <t>MPN or PN</t>
+  </si>
+  <si>
+    <t>T6620ORB OR 12584BIS</t>
+  </si>
+  <si>
+    <t>741WHNT OR JBC101</t>
+  </si>
+  <si>
+    <t>Brand Name or UPC</t>
+  </si>
+  <si>
+    <t>Jones Stephens OR 040688864563</t>
+  </si>
+  <si>
+    <t>Kohler OR 087206764776</t>
+  </si>
+  <si>
+    <t>879211400 OR K6589-U-K4</t>
+  </si>
+  <si>
+    <t>UPC or PN</t>
+  </si>
+  <si>
+    <t>040688864563 OR 63003LF-RB</t>
+  </si>
+  <si>
+    <t>Brizo AND 63003LF-RB</t>
+  </si>
+  <si>
+    <t>BN And MPN</t>
+  </si>
+  <si>
+    <t>Jones Stephens AND JBC102</t>
+  </si>
+  <si>
+    <t>Nutone AND 741SN</t>
   </si>
 </sst>
 </file>
@@ -1447,6 +1520,309 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="B1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
@@ -1581,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,45 +2010,45 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1048576"/>
+      <selection activeCell="B4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>6</v>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1683,107 +2059,128 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
+      <c r="B1" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>19</v>
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Search V2 Tests by making it more atomic
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="15" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="18" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="keyword_ExactMatch_PNOrMPN" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="keyword_OrCond_PNOrMPN" sheetId="10" r:id="rId7"/>
     <sheet name="keyword_OrCond_BNOrPN" sheetId="12" r:id="rId8"/>
     <sheet name="keyword_OrCond_MPNOrPN" sheetId="13" r:id="rId9"/>
-    <sheet name="keyword_OrCond_PNOrUPC" sheetId="14" r:id="rId10"/>
+    <sheet name="keyword_OrCond_UPCOrPN" sheetId="14" r:id="rId10"/>
     <sheet name="keyword_AndCond_BNAndMPN" sheetId="16" r:id="rId11"/>
     <sheet name="keyword_AndCond_PNAndMPN" sheetId="17" r:id="rId12"/>
     <sheet name="keyword_AndCond_BNAndPN" sheetId="18" r:id="rId13"/>
@@ -38,12 +38,12 @@
     <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId24"/>
     <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="87">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -51,18 +51,9 @@
     <t>TC_Searchv2_002</t>
   </si>
   <si>
-    <t>Part Number Or MPN</t>
-  </si>
-  <si>
-    <t>Brand Name Or UPC</t>
-  </si>
-  <si>
     <t>Brand Name Or Part Number</t>
   </si>
   <si>
-    <t>Brand Name Or MPN</t>
-  </si>
-  <si>
     <t>MPN</t>
   </si>
   <si>
@@ -105,81 +96,15 @@
     <t>087206579400</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   </t>
-  </si>
-  <si>
-    <t>Part Number or UPC</t>
-  </si>
-  <si>
-    <t>BainUltra ELEGANCIA7242C10BIS</t>
-  </si>
-  <si>
-    <t>ELEGANCIA7242C10WHT ELEGANCIA7242C10WHT</t>
-  </si>
-  <si>
-    <t>13861 K-7272-CP</t>
-  </si>
-  <si>
-    <t>Brizo 63003LF-RB</t>
-  </si>
-  <si>
-    <t>Nutone 026715145096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moen 026508161012 </t>
-  </si>
-  <si>
-    <t>Moen 026508161029</t>
-  </si>
-  <si>
-    <t>847877043767 800-12-B2-24</t>
-  </si>
-  <si>
-    <t>034449574501 T11800</t>
-  </si>
-  <si>
-    <t>TestUPC 12345</t>
-  </si>
-  <si>
     <t>BrandName or MPN</t>
   </si>
   <si>
-    <t>Gerber OR 649NS</t>
-  </si>
-  <si>
-    <t>Jones Stephens OR ELEGANCIA7242C10WHT</t>
-  </si>
-  <si>
-    <t>Aquatic  OR  2603-CTSR</t>
-  </si>
-  <si>
     <t>12584BIS OR T6620ORB</t>
   </si>
   <si>
     <t>JBC101 OR 741WHNT</t>
   </si>
   <si>
-    <t>Jones Stephens OR K6589-U-96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aquatic OR 2603CTSRWHT </t>
-  </si>
-  <si>
-    <t>BrandName or PN</t>
-  </si>
-  <si>
-    <t>MPN or PN</t>
-  </si>
-  <si>
-    <t>T6620ORB OR 12584BIS</t>
-  </si>
-  <si>
-    <t>741WHNT OR JBC101</t>
-  </si>
-  <si>
     <t>Brand Name or UPC</t>
   </si>
   <si>
@@ -189,118 +114,196 @@
     <t>Kohler OR 087206764776</t>
   </si>
   <si>
-    <t>879211400 OR K6589-U-K4</t>
-  </si>
-  <si>
-    <t>UPC or PN</t>
-  </si>
-  <si>
-    <t>040688864563 OR 63003LF-RB</t>
-  </si>
-  <si>
-    <t>Brizo AND 63003LF-RB</t>
-  </si>
-  <si>
-    <t>BN And MPN</t>
-  </si>
-  <si>
-    <t>Jones Stephens AND JBC102</t>
-  </si>
-  <si>
-    <t>Nutone AND 741SN</t>
-  </si>
-  <si>
     <t>TC_Searchv2_003</t>
   </si>
   <si>
-    <t>PN And MPN</t>
-  </si>
-  <si>
-    <t>K310-4M-BV AND K-310-4M-BV</t>
-  </si>
-  <si>
-    <t>4FIRECOLLAR AND STILCC400</t>
-  </si>
-  <si>
-    <t>STI AND 4FIRECOLLAR</t>
-  </si>
-  <si>
-    <t>BN And PN</t>
-  </si>
-  <si>
-    <t>Jones Stephens AND JBC103</t>
-  </si>
-  <si>
-    <t>BN And UPC</t>
-  </si>
-  <si>
-    <t>Jones Stephens AND 644132090760</t>
-  </si>
-  <si>
-    <t>Kohler AND 087206577666</t>
-  </si>
-  <si>
-    <t>PN And UPC</t>
-  </si>
-  <si>
-    <t>1607 AND 087206359736</t>
-  </si>
-  <si>
-    <t>K310-4M-BV AND 087206577666</t>
-  </si>
-  <si>
-    <t>BN - MPN</t>
-  </si>
-  <si>
-    <t>Kohler -K-6589-U-58</t>
-  </si>
-  <si>
-    <t>Jones Stephens -JBC102</t>
-  </si>
-  <si>
-    <t>ELEGANCIA7242C10BIS -STILCC300</t>
-  </si>
-  <si>
-    <t>PN - MPN</t>
-  </si>
-  <si>
-    <t>3860621VLBIS -STILCC200</t>
-  </si>
-  <si>
-    <t>BN - PN</t>
-  </si>
-  <si>
-    <t>Jones Stephens -JBC110</t>
-  </si>
-  <si>
-    <t>Jones Stephens -K-6589-U-58</t>
-  </si>
-  <si>
-    <t>BN - UPC</t>
-  </si>
-  <si>
-    <t>Jones Stephens -644132090746</t>
-  </si>
-  <si>
-    <t>Kohler -026508161012</t>
-  </si>
-  <si>
-    <t>MPN - PN</t>
-  </si>
-  <si>
-    <t>TestMPN -test1234</t>
-  </si>
-  <si>
-    <t>K-7104-BN -12345</t>
-  </si>
-  <si>
-    <t>UPC - PN</t>
-  </si>
-  <si>
-    <t>026508161029 -649NS</t>
-  </si>
-  <si>
-    <t>784891950148 -K-6589-U-58</t>
+    <t>Brand Name</t>
+  </si>
+  <si>
+    <t>BainUltra</t>
+  </si>
+  <si>
+    <t>ELEGANCIA7242C10BIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brizo </t>
+  </si>
+  <si>
+    <t>63003LF-RB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">026508161012 </t>
+  </si>
+  <si>
+    <t>026508161029</t>
+  </si>
+  <si>
+    <t>026715145096</t>
+  </si>
+  <si>
+    <t>800-12-B2-24</t>
+  </si>
+  <si>
+    <t>847877043767</t>
+  </si>
+  <si>
+    <t>T11800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestUPC </t>
+  </si>
+  <si>
+    <t>PartNumber</t>
+  </si>
+  <si>
+    <t>034449574501</t>
+  </si>
+  <si>
+    <t>649NS</t>
+  </si>
+  <si>
+    <t>2603-CTSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquatic  </t>
+  </si>
+  <si>
+    <t>Jones Stephens</t>
+  </si>
+  <si>
+    <t>Gerber</t>
+  </si>
+  <si>
+    <t>BrandName</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>12584BIS</t>
+  </si>
+  <si>
+    <t>JBC101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T6620ORB </t>
+  </si>
+  <si>
+    <t>741WHNT</t>
+  </si>
+  <si>
+    <t>K6589-U-96</t>
+  </si>
+  <si>
+    <t>2603CTSRWHT</t>
+  </si>
+  <si>
+    <t>Aquatic</t>
+  </si>
+  <si>
+    <t>879211400</t>
+  </si>
+  <si>
+    <t>K6589-U-K4</t>
+  </si>
+  <si>
+    <t>040688864563</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>JBC102</t>
+  </si>
+  <si>
+    <t>741SN</t>
+  </si>
+  <si>
+    <t>Brizo</t>
+  </si>
+  <si>
+    <t>Nutone</t>
+  </si>
+  <si>
+    <t>K-310-4M-BV</t>
+  </si>
+  <si>
+    <t>STILCC400</t>
+  </si>
+  <si>
+    <t>4FIRECOLLAR</t>
+  </si>
+  <si>
+    <t>K310-4M-BV</t>
+  </si>
+  <si>
+    <t>JBC103</t>
+  </si>
+  <si>
+    <t>STI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PN</t>
+  </si>
+  <si>
+    <t>644132090760</t>
+  </si>
+  <si>
+    <t>87206577666</t>
+  </si>
+  <si>
+    <t>Kohler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN </t>
+  </si>
+  <si>
+    <t>87206359736</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BN </t>
+  </si>
+  <si>
+    <t>K-6589-U-58</t>
+  </si>
+  <si>
+    <t>STILCC300</t>
+  </si>
+  <si>
+    <t>STILCC200</t>
+  </si>
+  <si>
+    <t>3860621VLBIS</t>
+  </si>
+  <si>
+    <t>JBC110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BN - </t>
+  </si>
+  <si>
+    <t>644132090746</t>
+  </si>
+  <si>
+    <t>026508161012</t>
+  </si>
+  <si>
+    <t>test1234</t>
+  </si>
+  <si>
+    <t>TestMPN</t>
+  </si>
+  <si>
+    <t>26508161029</t>
+  </si>
+  <si>
+    <t>784891950148</t>
   </si>
 </sst>
 </file>
@@ -359,7 +362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -397,11 +400,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -417,6 +433,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1586,32 +1615,42 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="1" customWidth="1"/>
-    <col min="3" max="242" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
+    <col min="4" max="242" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>25</v>
+      <c r="B3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1625,40 +1664,50 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>50</v>
+      <c r="B3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1669,48 +1718,61 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1721,40 +1783,50 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1765,40 +1837,50 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1809,40 +1891,50 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="48" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>64</v>
+        <v>71</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1853,40 +1945,50 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>66</v>
+        <v>23</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1607</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1897,40 +1999,50 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>70</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1941,40 +2053,50 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="C3" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>73</v>
+        <v>78</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1985,40 +2107,50 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2028,40 +2160,50 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>79</v>
+        <v>71</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2075,13 +2217,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2089,7 +2232,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2097,10 +2243,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2108,10 +2254,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2119,7 +2265,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2130,40 +2279,50 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>82</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2174,40 +2333,50 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>85</v>
+        <v>23</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2235,7 +2404,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2243,7 +2412,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2265,7 +2434,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,31 +2448,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2331,39 +2500,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2390,31 +2559,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2425,32 +2594,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2461,32 +2637,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2497,48 +2680,61 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2549,48 +2745,61 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2618,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2626,7 +2835,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2634,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2645,40 +2854,50 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2689,40 +2908,49 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>44</v>
+      <c r="B3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Multiple UOM Test cases
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -9,41 +9,55 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="18" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="24" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="keyword_ExactMatch_PNOrMPN" sheetId="1" r:id="rId1"/>
     <sheet name="keyword_ExactMatch_BNOrUPC" sheetId="2" r:id="rId2"/>
-    <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId3"/>
-    <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId4"/>
-    <sheet name="keyword_ExactMatching_UPCOrPN" sheetId="8" r:id="rId5"/>
-    <sheet name="keyword_OrCond_BrandNameOrMPN" sheetId="9" r:id="rId6"/>
-    <sheet name="keyword_OrCond_PNOrMPN" sheetId="10" r:id="rId7"/>
-    <sheet name="keyword_OrCond_BNOrPN" sheetId="12" r:id="rId8"/>
-    <sheet name="keyword_OrCond_MPNOrPN" sheetId="13" r:id="rId9"/>
-    <sheet name="keyword_OrCond_UPCOrPN" sheetId="14" r:id="rId10"/>
-    <sheet name="keyword_AndCond_BNAndMPN" sheetId="16" r:id="rId11"/>
-    <sheet name="keyword_AndCond_PNAndMPN" sheetId="17" r:id="rId12"/>
-    <sheet name="keyword_AndCond_BNAndPN" sheetId="18" r:id="rId13"/>
-    <sheet name="keyword_AndCond_BNAndUPC" sheetId="19" r:id="rId14"/>
-    <sheet name="keyword_AndCond_PNAndUPC" sheetId="20" r:id="rId15"/>
-    <sheet name="keyword_BNMinusMPN" sheetId="21" r:id="rId16"/>
-    <sheet name="keyword_PNMinusMPN" sheetId="22" r:id="rId17"/>
-    <sheet name="keyword_BNMinusPN" sheetId="23" r:id="rId18"/>
-    <sheet name="keyword_BNMinusUPC" sheetId="24" r:id="rId19"/>
-    <sheet name="keyword_MPNMinusPN" sheetId="25" r:id="rId20"/>
-    <sheet name="keyword_UPCMinusPN" sheetId="26" r:id="rId21"/>
-    <sheet name="keyword_OrCond_BNOrUPC" sheetId="15" r:id="rId22"/>
-    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId23"/>
-    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId24"/>
-    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId25"/>
+    <sheet name="keyword_BrandNamePlusMPN" sheetId="27" r:id="rId3"/>
+    <sheet name="keyword_PartNumberPlusMPN" sheetId="28" r:id="rId4"/>
+    <sheet name="keyword_BNPlusPN" sheetId="29" r:id="rId5"/>
+    <sheet name="keyword_BNPlusUPC" sheetId="30" r:id="rId6"/>
+    <sheet name="keyword_UPCPlusPN" sheetId="31" r:id="rId7"/>
+    <sheet name="keyword_partNumberNOTMpn" sheetId="34" r:id="rId8"/>
+    <sheet name="keyword_brandNameNOTPn" sheetId="35" r:id="rId9"/>
+    <sheet name="keyword_brandNameNOTUpc" sheetId="36" r:id="rId10"/>
+    <sheet name="keyword_uPCNOTPn" sheetId="37" r:id="rId11"/>
+    <sheet name="keyword_Parenthesis" sheetId="32" r:id="rId12"/>
+    <sheet name="keyword_BrandNameNOTMpn" sheetId="33" r:id="rId13"/>
+    <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId14"/>
+    <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId15"/>
+    <sheet name="keyword_ExactMatching_UPCOrPN" sheetId="8" r:id="rId16"/>
+    <sheet name="keyword_OrCond_BrandNameOrMPN" sheetId="9" r:id="rId17"/>
+    <sheet name="keyword_OrCond_PNOrMPN" sheetId="10" r:id="rId18"/>
+    <sheet name="keyword_OrCond_BNOrPN" sheetId="12" r:id="rId19"/>
+    <sheet name="keyword_OrCond_MPNOrPN" sheetId="13" r:id="rId20"/>
+    <sheet name="keyword_OrCond_UPCOrPN" sheetId="14" r:id="rId21"/>
+    <sheet name="keyword_AndCond_BNAndMPN" sheetId="16" r:id="rId22"/>
+    <sheet name="keyword_AndCond_PNAndMPN" sheetId="17" r:id="rId23"/>
+    <sheet name="keyword_AndCond_BNAndPN" sheetId="18" r:id="rId24"/>
+    <sheet name="keyword_AndCond_BNAndUPC" sheetId="19" r:id="rId25"/>
+    <sheet name="partialPNSearch_SKU" sheetId="38" r:id="rId26"/>
+    <sheet name="partialPNSearch_ProductMode" sheetId="39" r:id="rId27"/>
+    <sheet name="partialShortDescriptionSearch" sheetId="40" r:id="rId28"/>
+    <sheet name="keyword_AndCond_PNAndUPC" sheetId="20" r:id="rId29"/>
+    <sheet name="keyword_BNMinusMPN" sheetId="21" r:id="rId30"/>
+    <sheet name="keyword_PNMinusMPN" sheetId="22" r:id="rId31"/>
+    <sheet name="keyword_BNMinusPN" sheetId="23" r:id="rId32"/>
+    <sheet name="keyword_BNMinusUPC" sheetId="24" r:id="rId33"/>
+    <sheet name="keyword_MPNMinusPN" sheetId="25" r:id="rId34"/>
+    <sheet name="keyword_UPCMinusPN" sheetId="26" r:id="rId35"/>
+    <sheet name="keyword_OrCond_BNOrUPC" sheetId="15" r:id="rId36"/>
+    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId37"/>
+    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId38"/>
+    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId39"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="110">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -51,9 +65,6 @@
     <t>TC_Searchv2_002</t>
   </si>
   <si>
-    <t>Brand Name Or Part Number</t>
-  </si>
-  <si>
     <t>MPN</t>
   </si>
   <si>
@@ -126,9 +137,6 @@
     <t>ELEGANCIA7242C10BIS</t>
   </si>
   <si>
-    <t xml:space="preserve">Brizo </t>
-  </si>
-  <si>
     <t>63003LF-RB</t>
   </si>
   <si>
@@ -255,18 +263,12 @@
     <t>644132090760</t>
   </si>
   <si>
-    <t>87206577666</t>
-  </si>
-  <si>
     <t>Kohler</t>
   </si>
   <si>
     <t xml:space="preserve">PN </t>
   </si>
   <si>
-    <t>87206359736</t>
-  </si>
-  <si>
     <t xml:space="preserve">BN </t>
   </si>
   <si>
@@ -300,17 +302,98 @@
     <t>TestMPN</t>
   </si>
   <si>
-    <t>26508161029</t>
-  </si>
-  <si>
     <t>784891950148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JBC110 </t>
+  </si>
+  <si>
+    <t>12-584WHT</t>
+  </si>
+  <si>
+    <t>2603-CTSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12584BIS </t>
+  </si>
+  <si>
+    <t>011-2394-96</t>
+  </si>
+  <si>
+    <t>087206359736</t>
+  </si>
+  <si>
+    <t>650531846716</t>
+  </si>
+  <si>
+    <t>Parenthesis</t>
+  </si>
+  <si>
+    <t>"1/2 Inch MIP x FIP, 36 Inch L, 1/2 Inch psi, -40 to 150 deg F,"</t>
+  </si>
+  <si>
+    <t>"BOOTZ&amp;Reg; Syniron 2 011-2394 Soaking"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JBC102 </t>
+  </si>
+  <si>
+    <t>testMPN</t>
+  </si>
+  <si>
+    <t>BOOTZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STILCC200 </t>
+  </si>
+  <si>
+    <t>Brand name</t>
+  </si>
+  <si>
+    <t>650531148889</t>
+  </si>
+  <si>
+    <t xml:space="preserve">644132090722 </t>
+  </si>
+  <si>
+    <t>644132090722</t>
+  </si>
+  <si>
+    <t xml:space="preserve">730573039021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">649BZ </t>
+  </si>
+  <si>
+    <t>T6620BN</t>
+  </si>
+  <si>
+    <t>087206577666</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>K6589-U</t>
+  </si>
+  <si>
+    <t>Tset_Description</t>
+  </si>
+  <si>
+    <t>-40 to 150 deg F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -332,6 +415,11 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -439,13 +527,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1609,7 +1695,7 @@
   <dimension ref="A1:IH3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1625,10 +1711,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1636,10 +1722,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1647,10 +1733,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1667,6 +1753,673 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1682,10 +2435,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,10 +2446,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,10 +2457,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1716,7 +2469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1736,10 +2489,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1747,10 +2500,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1758,10 +2511,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1769,10 +2522,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1781,7 +2534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1801,32 +2554,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1835,7 +2588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1855,32 +2608,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1889,12 +2642,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,32 +2662,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1943,12 +2696,124 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,32 +2828,85 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="19">
-        <v>1607</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>73</v>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1997,7 +2915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2017,32 +2935,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2051,7 +2969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2070,33 +2988,33 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>46</v>
+      <c r="B1" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2105,7 +3023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2125,40 +3043,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2178,32 +3096,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2212,72 +3130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2297,32 +3150,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2331,12 +3184,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,32 +3204,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2385,7 +3238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2404,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2412,7 +3265,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2420,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2429,7 +3282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2448,31 +3301,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2481,7 +3334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2500,47 +3353,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2559,31 +3412,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2592,19 +3445,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2612,53 +3465,62 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+      <c r="B2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>3</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2666,140 +3528,126 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+        <v>42</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>38</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>34</v>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>3</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>40</v>
+      <c r="B2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>41</v>
+      <c r="B3" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2808,74 +3656,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>46</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2883,10 +3686,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>92</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2894,15 +3697,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+        <v>86</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2911,24 +3713,24 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>46</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2936,25 +3738,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code of Etna with search v2 bug fixed and adding normalize space for clicking on created cart and created my product group
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -9,55 +9,61 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="24" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="keyword_ExactMatch_PNOrMPN" sheetId="1" r:id="rId1"/>
-    <sheet name="keyword_ExactMatch_BNOrUPC" sheetId="2" r:id="rId2"/>
-    <sheet name="keyword_BrandNamePlusMPN" sheetId="27" r:id="rId3"/>
-    <sheet name="keyword_PartNumberPlusMPN" sheetId="28" r:id="rId4"/>
-    <sheet name="keyword_BNPlusPN" sheetId="29" r:id="rId5"/>
-    <sheet name="keyword_BNPlusUPC" sheetId="30" r:id="rId6"/>
-    <sheet name="keyword_UPCPlusPN" sheetId="31" r:id="rId7"/>
-    <sheet name="keyword_partNumberNOTMpn" sheetId="34" r:id="rId8"/>
-    <sheet name="keyword_brandNameNOTPn" sheetId="35" r:id="rId9"/>
-    <sheet name="keyword_brandNameNOTUpc" sheetId="36" r:id="rId10"/>
-    <sheet name="keyword_uPCNOTPn" sheetId="37" r:id="rId11"/>
-    <sheet name="keyword_Parenthesis" sheetId="32" r:id="rId12"/>
-    <sheet name="keyword_BrandNameNOTMpn" sheetId="33" r:id="rId13"/>
-    <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId14"/>
-    <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId15"/>
-    <sheet name="keyword_ExactMatching_UPCOrPN" sheetId="8" r:id="rId16"/>
-    <sheet name="keyword_OrCond_BrandNameOrMPN" sheetId="9" r:id="rId17"/>
-    <sheet name="keyword_OrCond_PNOrMPN" sheetId="10" r:id="rId18"/>
-    <sheet name="keyword_OrCond_BNOrPN" sheetId="12" r:id="rId19"/>
-    <sheet name="keyword_OrCond_MPNOrPN" sheetId="13" r:id="rId20"/>
-    <sheet name="keyword_OrCond_UPCOrPN" sheetId="14" r:id="rId21"/>
-    <sheet name="keyword_AndCond_BNAndMPN" sheetId="16" r:id="rId22"/>
-    <sheet name="keyword_AndCond_PNAndMPN" sheetId="17" r:id="rId23"/>
-    <sheet name="keyword_AndCond_BNAndPN" sheetId="18" r:id="rId24"/>
-    <sheet name="keyword_AndCond_BNAndUPC" sheetId="19" r:id="rId25"/>
-    <sheet name="partialPNSearch_SKU" sheetId="38" r:id="rId26"/>
-    <sheet name="partialPNSearch_ProductMode" sheetId="39" r:id="rId27"/>
-    <sheet name="partialShortDescriptionSearch" sheetId="40" r:id="rId28"/>
-    <sheet name="keyword_AndCond_PNAndUPC" sheetId="20" r:id="rId29"/>
-    <sheet name="keyword_BNMinusMPN" sheetId="21" r:id="rId30"/>
-    <sheet name="keyword_PNMinusMPN" sheetId="22" r:id="rId31"/>
-    <sheet name="keyword_BNMinusPN" sheetId="23" r:id="rId32"/>
-    <sheet name="keyword_BNMinusUPC" sheetId="24" r:id="rId33"/>
-    <sheet name="keyword_MPNMinusPN" sheetId="25" r:id="rId34"/>
-    <sheet name="keyword_UPCMinusPN" sheetId="26" r:id="rId35"/>
-    <sheet name="keyword_OrCond_BNOrUPC" sheetId="15" r:id="rId36"/>
-    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId37"/>
-    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId38"/>
-    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId39"/>
+    <sheet name="Sheet4" sheetId="46" r:id="rId1"/>
+    <sheet name="keyword_ExactMatch_PNOrMPN" sheetId="1" r:id="rId2"/>
+    <sheet name="keyword_ExactMatch_BNOrUPC" sheetId="2" r:id="rId3"/>
+    <sheet name="keyword_BrandNamePlusMPN" sheetId="27" r:id="rId4"/>
+    <sheet name="keyword_PartNumberPlusMPN" sheetId="28" r:id="rId5"/>
+    <sheet name="keyword_BNPlusPN" sheetId="29" r:id="rId6"/>
+    <sheet name="keyword_BNPlusUPC" sheetId="30" r:id="rId7"/>
+    <sheet name="keyword_UPCPlusPN" sheetId="31" r:id="rId8"/>
+    <sheet name="keyword_partNumberNOTMpn" sheetId="34" r:id="rId9"/>
+    <sheet name="keyword_brandNameNOTPn" sheetId="35" r:id="rId10"/>
+    <sheet name="keyword_brandNameNOTUpc" sheetId="36" r:id="rId11"/>
+    <sheet name="keyword_uPCNOTPn" sheetId="37" r:id="rId12"/>
+    <sheet name="keyword_Parenthesis" sheetId="32" r:id="rId13"/>
+    <sheet name="keyword_BrandNameNOTMpn" sheetId="33" r:id="rId14"/>
+    <sheet name="keyword_ExactMatch_BNOrPN" sheetId="3" r:id="rId15"/>
+    <sheet name="keyword_ExactMatching_BNOrMPN" sheetId="4" r:id="rId16"/>
+    <sheet name="keyword_ExactMatching_UPCOrPN" sheetId="8" r:id="rId17"/>
+    <sheet name="keyword_OrCond_BrandNameOrMPN" sheetId="9" r:id="rId18"/>
+    <sheet name="keyword_OrCond_PNOrMPN" sheetId="10" r:id="rId19"/>
+    <sheet name="keyword_OrCond_BNOrPN" sheetId="12" r:id="rId20"/>
+    <sheet name="keyword_OrCond_MPNOrPN" sheetId="13" r:id="rId21"/>
+    <sheet name="keyword_OrCond_UPCOrPN" sheetId="14" r:id="rId22"/>
+    <sheet name="keyword_AndCond_BNAndMPN" sheetId="16" r:id="rId23"/>
+    <sheet name="keyword_AndCond_PNAndMPN" sheetId="17" r:id="rId24"/>
+    <sheet name="keyword_AndCond_BNAndPN" sheetId="18" r:id="rId25"/>
+    <sheet name="keyword_AndCond_BNAndUPC" sheetId="19" r:id="rId26"/>
+    <sheet name="partialPNSearch_SKU" sheetId="38" r:id="rId27"/>
+    <sheet name="partialPNSearch_ProductMode" sheetId="39" r:id="rId28"/>
+    <sheet name="partialShortDescriptionSearch" sheetId="40" r:id="rId29"/>
+    <sheet name="fullShortDescriptionSearch" sheetId="41" r:id="rId30"/>
+    <sheet name="categoryNamesLastLevel" sheetId="42" r:id="rId31"/>
+    <sheet name="categoryNamesExceptLastLevel" sheetId="43" r:id="rId32"/>
+    <sheet name="autoSuggest" sheetId="44" r:id="rId33"/>
+    <sheet name="partialAutoSuggest" sheetId="45" r:id="rId34"/>
+    <sheet name="keyword_AndCond_PNAndUPC" sheetId="20" r:id="rId35"/>
+    <sheet name="keyword_BNMinusMPN" sheetId="21" r:id="rId36"/>
+    <sheet name="keyword_PNMinusMPN" sheetId="22" r:id="rId37"/>
+    <sheet name="keyword_BNMinusPN" sheetId="23" r:id="rId38"/>
+    <sheet name="keyword_BNMinusUPC" sheetId="24" r:id="rId39"/>
+    <sheet name="keyword_MPNMinusPN" sheetId="25" r:id="rId40"/>
+    <sheet name="keyword_UPCMinusPN" sheetId="26" r:id="rId41"/>
+    <sheet name="keyword_OrCond_BNOrUPC" sheetId="15" r:id="rId42"/>
+    <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId43"/>
+    <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId44"/>
+    <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId45"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="129">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -387,13 +393,70 @@
   </si>
   <si>
     <t>-40 to 150 deg F</t>
+  </si>
+  <si>
+    <t>Partial Short Description</t>
+  </si>
+  <si>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>Kohler® Karbon® Contemporary K-6227-C11 Articulating Kitchen Sink Faucet, Residential, 1.8 gpm, Polished Chrome</t>
+  </si>
+  <si>
+    <t>Delta® Cassidy™ T11897 3-Function Diverter Valve Trim without Handle, 1-Handle, Wall Mount, Brass, Chrome</t>
+  </si>
+  <si>
+    <t>Category Names</t>
+  </si>
+  <si>
+    <t>Bathroom Vanities</t>
+  </si>
+  <si>
+    <t>Bathroom Vanity Accessories</t>
+  </si>
+  <si>
+    <t>Sinks &amp; Lavatories</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>Bath/Showers</t>
+  </si>
+  <si>
+    <t>Search Text</t>
+  </si>
+  <si>
+    <t>Gas Line Connectors</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Partial Search Text</t>
+  </si>
+  <si>
+    <t>Expected Category to Come in the dropdown</t>
+  </si>
+  <si>
+    <t>plu</t>
+  </si>
+  <si>
+    <t>Plumbing Drains</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -419,6 +482,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -505,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -532,6 +601,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1692,10 +1780,571 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IH3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1748,502 +2397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2297,7 +2451,453 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -2362,18 +2962,266 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2381,183 +3229,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2567,19 +3242,19 @@
       <c r="B2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>60</v>
+      <c r="C2" s="16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>61</v>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2588,19 +3263,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2608,10 +3283,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2619,10 +3294,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2633,7 +3308,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2642,30 +3317,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+      <selection activeCell="C3" sqref="B2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>5</v>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2673,10 +3348,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>67</v>
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2684,10 +3359,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>74</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2696,131 +3371,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2828,10 +3391,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2839,95 +3402,41 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>103</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2935,10 +3444,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>2</v>
+        <v>55</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2946,10 +3455,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2957,10 +3466,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>56</v>
+        <v>68</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2969,30 +3478,83 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="B2:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3000,10 +3562,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3011,10 +3573,10 @@
         <v>22</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>73</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3023,19 +3585,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3043,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>44</v>
@@ -3053,19 +3615,19 @@
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>41</v>
+      <c r="B2" s="17" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>41</v>
+      <c r="B3" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>71</v>
@@ -3073,172 +3635,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3282,7 +3683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3334,7 +3735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -3393,7 +3794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3445,7 +3846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3498,7 +3899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3550,7 +3951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3603,7 +4004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3656,7 +4057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3706,56 +4107,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added geckodriver(marionette). Added narrow general search -> attribute narrow search scenario
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/SearchV2.xlsx
+++ b/resources/ExcelsheetData/SearchV2.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\Etna\resources\ExcelsheetData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="11760" tabRatio="866" firstSheet="47" activeTab="51"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="46" r:id="rId1"/>
@@ -63,13 +58,14 @@
     <sheet name="keywords_exactMatching_MPN" sheetId="5" r:id="rId49"/>
     <sheet name="keywords_exactMatching_PN" sheetId="6" r:id="rId50"/>
     <sheet name="keywords_exactMatching_UPC" sheetId="7" r:id="rId51"/>
+    <sheet name="searchWithinAttributeName" sheetId="53" r:id="rId52"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="161">
   <si>
     <t xml:space="preserve">TC No </t>
   </si>
@@ -502,12 +498,63 @@
   <si>
     <t>*41WHNT*</t>
   </si>
+  <si>
+    <t>Filter Name</t>
+  </si>
+  <si>
+    <t>Attribute Name</t>
+  </si>
+  <si>
+    <t>Firestop Collars</t>
+  </si>
+  <si>
+    <t>Expansion Begins</t>
+  </si>
+  <si>
+    <t>Strainers</t>
+  </si>
+  <si>
+    <t>Fan Light Combinations</t>
+  </si>
+  <si>
+    <t>Amperage Rating</t>
+  </si>
+  <si>
+    <t>2.2 A</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Celcon Trim, Plastic Base</t>
+  </si>
+  <si>
+    <t>320 deg F</t>
+  </si>
+  <si>
+    <t>Escutcheons</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>1-1/2 Inch ID x 3 Inch OD</t>
+  </si>
+  <si>
+    <t>Bar Sinks</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Almond</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -625,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -671,6 +718,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1830,34 +1879,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1868,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1879,7 +1928,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1897,21 +1946,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1922,7 +1971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1933,7 +1982,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1950,20 +1999,20 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +2023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1985,7 +2034,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2002,21 +2051,21 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2038,7 +2087,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2055,20 +2104,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2079,7 +2128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2090,7 +2139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2108,20 +2157,20 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2143,7 +2192,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2160,20 +2209,20 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2184,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2195,7 +2244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2212,20 +2261,20 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2236,7 +2285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2247,7 +2296,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2264,21 +2313,21 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2338,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2300,7 +2349,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2317,20 +2366,20 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2387,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2346,7 +2395,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2361,21 +2410,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2386,7 +2435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -2397,7 +2446,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -2408,7 +2457,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -2426,20 +2475,20 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2450,7 +2499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2461,7 +2510,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2472,7 +2521,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2490,21 +2539,21 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2515,7 +2564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2526,7 +2575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2537,7 +2586,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2555,21 +2604,21 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2580,7 +2629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2598,21 +2647,21 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2623,7 +2672,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2634,7 +2683,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2645,7 +2694,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2663,21 +2712,21 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2688,7 +2737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2699,7 +2748,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2710,7 +2759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2728,20 +2777,20 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2757,7 +2806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2772,21 +2821,21 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2846,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2808,7 +2857,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2826,20 +2875,20 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2850,7 +2899,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2861,7 +2910,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2879,21 +2928,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2904,7 +2953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2915,7 +2964,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2933,21 +2982,21 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2958,7 +3007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -2969,7 +3018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -2980,7 +3029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2998,21 +3047,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3023,7 +3072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -3034,7 +3083,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -3052,21 +3101,21 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3077,7 +3126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3088,7 +3137,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3106,21 +3155,21 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3131,7 +3180,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3142,7 +3191,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3160,21 +3209,21 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3185,7 +3234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3196,7 +3245,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3214,19 +3263,19 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3234,7 +3283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
         <v>104</v>
       </c>
@@ -3249,20 +3298,20 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3270,7 +3319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
         <v>104</v>
       </c>
@@ -3284,19 +3333,19 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3304,7 +3353,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
         <v>104</v>
       </c>
@@ -3312,7 +3361,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
         <v>105</v>
       </c>
@@ -3326,19 +3375,19 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3346,7 +3395,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="45">
       <c r="A2" s="22" t="s">
         <v>104</v>
       </c>
@@ -3354,7 +3403,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="45">
       <c r="A3" s="22" t="s">
         <v>105</v>
       </c>
@@ -3369,19 +3418,19 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -3389,7 +3438,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16.5" customHeight="1">
       <c r="A2" s="26" t="s">
         <v>104</v>
       </c>
@@ -3397,7 +3446,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1">
       <c r="A3" s="26" t="s">
         <v>105</v>
       </c>
@@ -3405,7 +3454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="26" t="s">
         <v>119</v>
       </c>
@@ -3420,19 +3469,19 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -3440,7 +3489,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="26" t="s">
         <v>104</v>
       </c>
@@ -3454,19 +3503,19 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -3474,7 +3523,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="26" t="s">
         <v>104</v>
       </c>
@@ -3482,7 +3531,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="26" t="s">
         <v>105</v>
       </c>
@@ -3490,7 +3539,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="26" t="s">
         <v>118</v>
       </c>
@@ -3498,7 +3547,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="26" t="s">
         <v>119</v>
       </c>
@@ -3506,7 +3555,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="26" t="s">
         <v>123</v>
       </c>
@@ -3521,21 +3570,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3546,7 +3595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -3557,7 +3606,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -3575,20 +3624,20 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -3599,7 +3648,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="26" t="s">
         <v>104</v>
       </c>
@@ -3610,7 +3659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="26" t="s">
         <v>104</v>
       </c>
@@ -3627,21 +3676,21 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3652,7 +3701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3663,7 +3712,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3681,21 +3730,21 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3706,7 +3755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3717,7 +3766,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3735,21 +3784,21 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3760,7 +3809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3771,7 +3820,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3789,21 +3838,21 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3814,7 +3863,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3825,7 +3874,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3842,21 +3891,21 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3867,7 +3916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3878,7 +3927,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3896,21 +3945,21 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3921,7 +3970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3932,7 +3981,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -3950,21 +3999,21 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3975,7 +4024,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -3986,7 +4035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -4004,20 +4053,20 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4025,7 +4074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -4033,7 +4082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -4048,20 +4097,20 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4069,7 +4118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -4077,7 +4126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -4085,7 +4134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -4100,21 +4149,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4125,7 +4174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -4142,20 +4191,20 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4163,7 +4212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -4171,7 +4220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -4179,7 +4228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -4187,7 +4236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -4201,20 +4250,20 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+      <selection activeCell="B4" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4222,7 +4271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -4230,7 +4279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -4238,7 +4287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4252,21 +4301,127 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4277,7 +4432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -4294,21 +4449,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4474,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -4336,14 +4491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IH3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" style="1" customWidth="1"/>
@@ -4351,7 +4506,7 @@
     <col min="4" max="242" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4362,7 +4517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -4373,7 +4528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -4394,21 +4549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4419,7 +4574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -4430,7 +4585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -4441,7 +4596,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>

</xml_diff>